<commit_message>
old kidney results, new plots for scc_p5
</commit_message>
<xml_diff>
--- a/results/summary files/rep1_run1/all_results.xlsx
+++ b/results/summary files/rep1_run1/all_results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="20">
   <si>
     <t>artificial_uniform_distinct</t>
   </si>
@@ -9171,6 +9171,169 @@
         <v>0.61</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65"/>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.882041761053729</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.8826079562193381</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.9179191506358779</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.8853453459031966</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.8759874626340003</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="n">
+        <v>2.444914051816823</v>
+      </c>
+      <c r="C67" t="n">
+        <v>2.548776716957037</v>
+      </c>
+      <c r="D67" t="n">
+        <v>2.0235906875439844</v>
+      </c>
+      <c r="E67" t="n">
+        <v>2.2829123450279694</v>
+      </c>
+      <c r="F67" t="n">
+        <v>2.4243985502573473</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F69" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>11</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
updated rep1_run1 results because RMSE calculation changed
</commit_message>
<xml_diff>
--- a/results/summary files/rep1_run1/all_results.xlsx
+++ b/results/summary files/rep1_run1/all_results.xlsx
@@ -176,19 +176,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1.2926947619533717</v>
+        <v>0.03785268947643256</v>
       </c>
       <c r="C4" t="n">
-        <v>1.3859860718551997</v>
+        <v>0.043853733180748575</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9811253088233477</v>
+        <v>0.028069793145086615</v>
       </c>
       <c r="E4" t="n">
-        <v>1.0933122654904244</v>
+        <v>0.03175566802317096</v>
       </c>
       <c r="F4" t="n">
-        <v>2.1750538079281507</v>
+        <v>0.06592204425902984</v>
       </c>
     </row>
     <row r="5">
@@ -339,19 +339,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>1.5350245172727026</v>
+        <v>0.04547222055136658</v>
       </c>
       <c r="C13" t="n">
-        <v>1.4945036264496134</v>
+        <v>0.04683728363013155</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9429557545191501</v>
+        <v>0.02597558522986028</v>
       </c>
       <c r="E13" t="n">
-        <v>1.078111957261458</v>
+        <v>0.031180174701324257</v>
       </c>
       <c r="F13" t="n">
-        <v>1.4987540875841094</v>
+        <v>0.04478674263149849</v>
       </c>
     </row>
     <row r="14">
@@ -502,19 +502,19 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>1.5961460095563285</v>
+        <v>0.0507241657831936</v>
       </c>
       <c r="C22" t="n">
-        <v>1.4943438734086458</v>
+        <v>0.048568162101392275</v>
       </c>
       <c r="D22" t="n">
-        <v>1.0596685210563987</v>
+        <v>0.03227331503834855</v>
       </c>
       <c r="E22" t="n">
-        <v>1.16546215945457</v>
+        <v>0.036386843069721765</v>
       </c>
       <c r="F22" t="n">
-        <v>1.4497420429868615</v>
+        <v>0.046613239995667216</v>
       </c>
     </row>
     <row r="23">
@@ -665,19 +665,19 @@
         <v>7</v>
       </c>
       <c r="B31" t="n">
-        <v>1.557397562291686</v>
+        <v>0.051297728887306146</v>
       </c>
       <c r="C31" t="n">
-        <v>1.337684544073257</v>
+        <v>0.0449190441538404</v>
       </c>
       <c r="D31" t="n">
-        <v>0.9594099500436091</v>
+        <v>0.028136349577425265</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9927351975226714</v>
+        <v>0.030728209898819792</v>
       </c>
       <c r="F31" t="n">
-        <v>1.369564001687953</v>
+        <v>0.04418980250131124</v>
       </c>
     </row>
     <row r="32">
@@ -828,19 +828,19 @@
         <v>7</v>
       </c>
       <c r="B40" t="n">
-        <v>2.9633552147316435</v>
+        <v>0.08817494901497673</v>
       </c>
       <c r="C40" t="n">
-        <v>1.0047179853666366</v>
+        <v>0.02984722483405088</v>
       </c>
       <c r="D40" t="n">
-        <v>0.6585117201259334</v>
+        <v>0.013252946409163562</v>
       </c>
       <c r="E40" t="n">
-        <v>0.936822173361457</v>
+        <v>0.02074074002476484</v>
       </c>
       <c r="F40" t="n">
-        <v>2.735960916342328</v>
+        <v>0.07455595160418878</v>
       </c>
     </row>
     <row r="41">
@@ -991,19 +991,19 @@
         <v>7</v>
       </c>
       <c r="B49" t="n">
-        <v>2.8102864776118293</v>
+        <v>0.0931391729351107</v>
       </c>
       <c r="C49" t="n">
-        <v>1.6233614266018053</v>
+        <v>0.05035194404431598</v>
       </c>
       <c r="D49" t="n">
-        <v>1.0493673194496007</v>
+        <v>0.028334358368999328</v>
       </c>
       <c r="E49" t="n">
-        <v>0.961645772383998</v>
+        <v>0.02657343115626215</v>
       </c>
       <c r="F49" t="n">
-        <v>3.049947573147447</v>
+        <v>0.0976660649745998</v>
       </c>
     </row>
     <row r="50">
@@ -1154,19 +1154,19 @@
         <v>7</v>
       </c>
       <c r="B58" t="n">
-        <v>1.5962618453671462</v>
+        <v>0.05170400173138735</v>
       </c>
       <c r="C58" t="n">
-        <v>1.4083250609117293</v>
+        <v>0.04814813336068909</v>
       </c>
       <c r="D58" t="n">
-        <v>0.8711891241880144</v>
+        <v>0.02620804523466258</v>
       </c>
       <c r="E58" t="n">
-        <v>0.9646127922311093</v>
+        <v>0.030455947915766536</v>
       </c>
       <c r="F58" t="n">
-        <v>1.5128055980050086</v>
+        <v>0.050044749060282216</v>
       </c>
     </row>
     <row r="59">
@@ -1317,19 +1317,19 @@
         <v>7</v>
       </c>
       <c r="B67" t="n">
-        <v>1.2570061705820563</v>
+        <v>0.039962151941329176</v>
       </c>
       <c r="C67" t="n">
-        <v>1.243285751024868</v>
+        <v>0.04255592717210191</v>
       </c>
       <c r="D67" t="n">
-        <v>0.8463930480727138</v>
+        <v>0.026219941249390755</v>
       </c>
       <c r="E67" t="n">
-        <v>0.9200382327037682</v>
+        <v>0.028918449190338733</v>
       </c>
       <c r="F67" t="n">
-        <v>1.2859671134849537</v>
+        <v>0.04316089902087136</v>
       </c>
     </row>
     <row r="68">
@@ -1493,19 +1493,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>5.078834915664358</v>
+        <v>0.15899872765453513</v>
       </c>
       <c r="C4" t="n">
-        <v>4.384929576155266</v>
+        <v>0.13179121851302375</v>
       </c>
       <c r="D4" t="n">
-        <v>2.488354267469829</v>
+        <v>0.05990288958625696</v>
       </c>
       <c r="E4" t="n">
-        <v>2.50720763748141</v>
+        <v>0.06913094069331736</v>
       </c>
       <c r="F4" t="n">
-        <v>2.460232450683747</v>
+        <v>0.059618315711254026</v>
       </c>
     </row>
     <row r="5">
@@ -1656,19 +1656,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>4.362172144645371</v>
+        <v>0.15249198937106806</v>
       </c>
       <c r="C13" t="n">
-        <v>2.989673830894909</v>
+        <v>0.09134901225440302</v>
       </c>
       <c r="D13" t="n">
-        <v>1.9866819775151552</v>
+        <v>0.048466993230758496</v>
       </c>
       <c r="E13" t="n">
-        <v>1.7130661613603475</v>
+        <v>0.042667226425681305</v>
       </c>
       <c r="F13" t="n">
-        <v>1.9306526191509894</v>
+        <v>0.04920134406892473</v>
       </c>
     </row>
     <row r="14">
@@ -1819,19 +1819,19 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>3.894173949705536</v>
+        <v>0.13568251716037494</v>
       </c>
       <c r="C22" t="n">
-        <v>2.9440954224159595</v>
+        <v>0.09538959298354645</v>
       </c>
       <c r="D22" t="n">
-        <v>2.6862487490249185</v>
+        <v>0.08025491662321808</v>
       </c>
       <c r="E22" t="n">
-        <v>2.9428965792784774</v>
+        <v>0.09194453877099783</v>
       </c>
       <c r="F22" t="n">
-        <v>3.0965336647692245</v>
+        <v>0.09649111789327293</v>
       </c>
     </row>
     <row r="23">
@@ -1982,19 +1982,19 @@
         <v>7</v>
       </c>
       <c r="B31" t="n">
-        <v>3.416470119661446</v>
+        <v>0.10578620633377983</v>
       </c>
       <c r="C31" t="n">
-        <v>3.6461322190877126</v>
+        <v>0.11219324994486829</v>
       </c>
       <c r="D31" t="n">
-        <v>2.5341543106552207</v>
+        <v>0.06831300000813174</v>
       </c>
       <c r="E31" t="n">
-        <v>2.157526330621538</v>
+        <v>0.05815133625206172</v>
       </c>
       <c r="F31" t="n">
-        <v>2.432350173819722</v>
+        <v>0.06582834649209358</v>
       </c>
     </row>
     <row r="32">
@@ -2145,19 +2145,19 @@
         <v>7</v>
       </c>
       <c r="B40" t="n">
-        <v>6.564462550508305</v>
+        <v>0.23735037542220022</v>
       </c>
       <c r="C40" t="n">
-        <v>1.432911357150496</v>
+        <v>0.04410701220038978</v>
       </c>
       <c r="D40" t="n">
-        <v>1.0661432508118187</v>
+        <v>0.019047545983160954</v>
       </c>
       <c r="E40" t="n">
-        <v>1.7806682830535758</v>
+        <v>0.03261952762932004</v>
       </c>
       <c r="F40" t="n">
-        <v>2.676063129931507</v>
+        <v>0.051957415320169835</v>
       </c>
     </row>
     <row r="41">
@@ -2308,19 +2308,19 @@
         <v>7</v>
       </c>
       <c r="B49" t="n">
-        <v>6.129656798995612</v>
+        <v>0.22161156679768557</v>
       </c>
       <c r="C49" t="n">
-        <v>3.0108411353724422</v>
+        <v>0.09490652743619438</v>
       </c>
       <c r="D49" t="n">
-        <v>2.0124316629542434</v>
+        <v>0.050971215899528764</v>
       </c>
       <c r="E49" t="n">
-        <v>1.7771310016307271</v>
+        <v>0.041874345337151675</v>
       </c>
       <c r="F49" t="n">
-        <v>2.1785480924094704</v>
+        <v>0.059452910817603614</v>
       </c>
     </row>
     <row r="50">
@@ -2471,19 +2471,19 @@
         <v>7</v>
       </c>
       <c r="B58" t="n">
-        <v>4.389543091259763</v>
+        <v>0.13605678116976308</v>
       </c>
       <c r="C58" t="n">
-        <v>4.048546869156876</v>
+        <v>0.12359755183944827</v>
       </c>
       <c r="D58" t="n">
-        <v>2.8919719333518428</v>
+        <v>0.07612321082488101</v>
       </c>
       <c r="E58" t="n">
-        <v>2.813012540735347</v>
+        <v>0.07746769192035494</v>
       </c>
       <c r="F58" t="n">
-        <v>3.0122798171550706</v>
+        <v>0.07928235044989738</v>
       </c>
     </row>
     <row r="59">
@@ -2634,19 +2634,19 @@
         <v>7</v>
       </c>
       <c r="B67" t="n">
-        <v>5.779854858938781</v>
+        <v>0.19428929003163647</v>
       </c>
       <c r="C67" t="n">
-        <v>3.32098104979115</v>
+        <v>0.09926760233126716</v>
       </c>
       <c r="D67" t="n">
-        <v>2.098420994899459</v>
+        <v>0.047147953445608175</v>
       </c>
       <c r="E67" t="n">
-        <v>1.6933303132673552</v>
+        <v>0.03640775963097928</v>
       </c>
       <c r="F67" t="n">
-        <v>2.1395566310193046</v>
+        <v>0.04855393722085318</v>
       </c>
     </row>
     <row r="68">
@@ -2810,19 +2810,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1.6497109082468475</v>
+        <v>0.04909033841863245</v>
       </c>
       <c r="C4" t="n">
-        <v>2.0170591935262987</v>
+        <v>0.06436912503493038</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7871373788433538</v>
+        <v>0.015737081804235584</v>
       </c>
       <c r="E4" t="n">
-        <v>1.7277184876543705</v>
+        <v>0.03653281912403025</v>
       </c>
       <c r="F4" t="n">
-        <v>1.9457789051131447</v>
+        <v>0.04341908040313372</v>
       </c>
     </row>
     <row r="5">
@@ -2973,19 +2973,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>3.0035388815124398</v>
+        <v>0.09702862655994468</v>
       </c>
       <c r="C13" t="n">
-        <v>2.188738594128398</v>
+        <v>0.070373415633005</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5991988898172775</v>
+        <v>0.009654746607369655</v>
       </c>
       <c r="E13" t="n">
-        <v>1.6922755931319233</v>
+        <v>0.02591562649616545</v>
       </c>
       <c r="F13" t="n">
-        <v>1.8354988723080206</v>
+        <v>0.03227168831748265</v>
       </c>
     </row>
     <row r="14">
@@ -3136,19 +3136,19 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>2.0050643731052573</v>
+        <v>0.06404644424922415</v>
       </c>
       <c r="C22" t="n">
-        <v>2.298615439952834</v>
+        <v>0.07493884900836655</v>
       </c>
       <c r="D22" t="n">
-        <v>1.3055680316092324</v>
+        <v>0.03606748472985253</v>
       </c>
       <c r="E22" t="n">
-        <v>3.775409439378781</v>
+        <v>0.11225409516173468</v>
       </c>
       <c r="F22" t="n">
-        <v>3.49819368963541</v>
+        <v>0.10800804737410466</v>
       </c>
     </row>
     <row r="23">
@@ -3299,19 +3299,19 @@
         <v>7</v>
       </c>
       <c r="B31" t="n">
-        <v>2.4552678861253083</v>
+        <v>0.0718042652207066</v>
       </c>
       <c r="C31" t="n">
-        <v>2.085268741893903</v>
+        <v>0.0657991789651881</v>
       </c>
       <c r="D31" t="n">
-        <v>1.1663496438080687</v>
+        <v>0.030526916648706458</v>
       </c>
       <c r="E31" t="n">
-        <v>2.5274996506617398</v>
+        <v>0.06309212768746937</v>
       </c>
       <c r="F31" t="n">
-        <v>2.7759503149017526</v>
+        <v>0.06835896498882492</v>
       </c>
     </row>
     <row r="32">
@@ -3462,19 +3462,19 @@
         <v>7</v>
       </c>
       <c r="B40" t="n">
-        <v>4.243186954757895</v>
+        <v>0.13485450738133584</v>
       </c>
       <c r="C40" t="n">
-        <v>2.052880291963206</v>
+        <v>0.06334568678012854</v>
       </c>
       <c r="D40" t="n">
-        <v>0.5890980545360165</v>
+        <v>0.009819463099579748</v>
       </c>
       <c r="E40" t="n">
-        <v>1.6622534670448736</v>
+        <v>0.025744563105230166</v>
       </c>
       <c r="F40" t="n">
-        <v>2.1281232527307723</v>
+        <v>0.0361819680117821</v>
       </c>
     </row>
     <row r="41">
@@ -3625,19 +3625,19 @@
         <v>7</v>
       </c>
       <c r="B49" t="n">
-        <v>4.92265018028224</v>
+        <v>0.15959013337617997</v>
       </c>
       <c r="C49" t="n">
-        <v>4.347138951403421</v>
+        <v>0.13318344329029286</v>
       </c>
       <c r="D49" t="n">
-        <v>0.9038412752330857</v>
+        <v>0.016648464589975952</v>
       </c>
       <c r="E49" t="n">
-        <v>2.5596109066472574</v>
+        <v>0.04929710745194045</v>
       </c>
       <c r="F49" t="n">
-        <v>2.870915063008019</v>
+        <v>0.0708177261007614</v>
       </c>
     </row>
     <row r="50">
@@ -3788,19 +3788,19 @@
         <v>7</v>
       </c>
       <c r="B58" t="n">
-        <v>2.4530876602305343</v>
+        <v>0.06509094038619587</v>
       </c>
       <c r="C58" t="n">
-        <v>2.0131204006400374</v>
+        <v>0.06617377086645694</v>
       </c>
       <c r="D58" t="n">
-        <v>0.869834113679271</v>
+        <v>0.02139064677050981</v>
       </c>
       <c r="E58" t="n">
-        <v>3.3989996322584433</v>
+        <v>0.08582310328555552</v>
       </c>
       <c r="F58" t="n">
-        <v>3.698893273528289</v>
+        <v>0.09506168062097298</v>
       </c>
     </row>
     <row r="59">
@@ -3951,19 +3951,19 @@
         <v>7</v>
       </c>
       <c r="B67" t="n">
-        <v>2.6329059032869915</v>
+        <v>0.07374511984607748</v>
       </c>
       <c r="C67" t="n">
-        <v>2.1004506089673236</v>
+        <v>0.06511495532312823</v>
       </c>
       <c r="D67" t="n">
-        <v>0.8182791065266027</v>
+        <v>0.015051460702173539</v>
       </c>
       <c r="E67" t="n">
-        <v>1.4894161401007566</v>
+        <v>0.02660249442016389</v>
       </c>
       <c r="F67" t="n">
-        <v>1.8442431631416853</v>
+        <v>0.04003845712156537</v>
       </c>
     </row>
     <row r="68">
@@ -4127,19 +4127,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>3.0810941746434666</v>
+        <v>0.09944602702583323</v>
       </c>
       <c r="C4" t="n">
-        <v>2.055330967758803</v>
+        <v>0.07044993140345074</v>
       </c>
       <c r="D4" t="n">
-        <v>1.7120919283573957</v>
+        <v>0.05109466531947037</v>
       </c>
       <c r="E4" t="n">
-        <v>2.058925416347708</v>
+        <v>0.068962646947875</v>
       </c>
       <c r="F4" t="n">
-        <v>2.901476769000473</v>
+        <v>0.0916703406763285</v>
       </c>
     </row>
     <row r="5">
@@ -4290,19 +4290,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>2.200430485241284</v>
+        <v>0.07537160825214526</v>
       </c>
       <c r="C13" t="n">
-        <v>1.9788576069365154</v>
+        <v>0.06992124628672747</v>
       </c>
       <c r="D13" t="n">
-        <v>1.6610924543559464</v>
+        <v>0.05277109742515236</v>
       </c>
       <c r="E13" t="n">
-        <v>1.68012834965625</v>
+        <v>0.055486763459781804</v>
       </c>
       <c r="F13" t="n">
-        <v>1.959919543245863</v>
+        <v>0.06538817506271444</v>
       </c>
     </row>
     <row r="14">
@@ -4453,19 +4453,19 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>2.543498437988817</v>
+        <v>0.09211321423793466</v>
       </c>
       <c r="C22" t="n">
-        <v>1.9300123706987926</v>
+        <v>0.07009814417445753</v>
       </c>
       <c r="D22" t="n">
-        <v>1.941117065634486</v>
+        <v>0.06929601388648249</v>
       </c>
       <c r="E22" t="n">
-        <v>1.845489677282257</v>
+        <v>0.06601695335582487</v>
       </c>
       <c r="F22" t="n">
-        <v>2.249163197158759</v>
+        <v>0.07998730983508096</v>
       </c>
     </row>
     <row r="23">
@@ -4616,19 +4616,19 @@
         <v>7</v>
       </c>
       <c r="B31" t="n">
-        <v>2.809340470230682</v>
+        <v>0.09437968565517343</v>
       </c>
       <c r="C31" t="n">
-        <v>2.0038543339206494</v>
+        <v>0.07237858464572436</v>
       </c>
       <c r="D31" t="n">
-        <v>1.9577172021607565</v>
+        <v>0.06610634287039036</v>
       </c>
       <c r="E31" t="n">
-        <v>1.7464904224155975</v>
+        <v>0.05986983052172356</v>
       </c>
       <c r="F31" t="n">
-        <v>2.2011338050621654</v>
+        <v>0.0738913100707976</v>
       </c>
     </row>
     <row r="32">
@@ -4779,19 +4779,19 @@
         <v>7</v>
       </c>
       <c r="B40" t="n">
-        <v>4.874789817128091</v>
+        <v>0.1730541406521035</v>
       </c>
       <c r="C40" t="n">
-        <v>2.8511986014100867</v>
+        <v>0.09722853699494727</v>
       </c>
       <c r="D40" t="n">
-        <v>3.0462857148122247</v>
+        <v>0.098446888597617</v>
       </c>
       <c r="E40" t="n">
-        <v>1.9093414833186952</v>
+        <v>0.06354584879123705</v>
       </c>
       <c r="F40" t="n">
-        <v>4.64276673329566</v>
+        <v>0.15927017457771042</v>
       </c>
     </row>
     <row r="41">
@@ -4942,19 +4942,19 @@
         <v>7</v>
       </c>
       <c r="B49" t="n">
-        <v>5.190529131113787</v>
+        <v>0.16564267616789777</v>
       </c>
       <c r="C49" t="n">
-        <v>2.605458065463479</v>
+        <v>0.07761889776525806</v>
       </c>
       <c r="D49" t="n">
-        <v>3.358406309510313</v>
+        <v>0.09567943720600774</v>
       </c>
       <c r="E49" t="n">
-        <v>1.7810134468249188</v>
+        <v>0.04743648941493894</v>
       </c>
       <c r="F49" t="n">
-        <v>3.8594741762160205</v>
+        <v>0.10557040173598717</v>
       </c>
     </row>
     <row r="50">
@@ -5105,19 +5105,19 @@
         <v>7</v>
       </c>
       <c r="B58" t="n">
-        <v>2.504767237159626</v>
+        <v>0.0767557887887305</v>
       </c>
       <c r="C58" t="n">
-        <v>2.057493478968896</v>
+        <v>0.06642562671332232</v>
       </c>
       <c r="D58" t="n">
-        <v>1.7348118800040806</v>
+        <v>0.049175340261262676</v>
       </c>
       <c r="E58" t="n">
-        <v>1.8340303431127203</v>
+        <v>0.053869213379485234</v>
       </c>
       <c r="F58" t="n">
-        <v>2.169675071111345</v>
+        <v>0.06226395264064198</v>
       </c>
     </row>
     <row r="59">
@@ -5268,19 +5268,19 @@
         <v>7</v>
       </c>
       <c r="B67" t="n">
-        <v>3.3358710123775306</v>
+        <v>0.09992556959329578</v>
       </c>
       <c r="C67" t="n">
-        <v>2.29491047544149</v>
+        <v>0.07307332311279345</v>
       </c>
       <c r="D67" t="n">
-        <v>2.3395073180874766</v>
+        <v>0.06879159507579634</v>
       </c>
       <c r="E67" t="n">
-        <v>1.7601333009280644</v>
+        <v>0.052452782338620996</v>
       </c>
       <c r="F67" t="n">
-        <v>2.519035044769759</v>
+        <v>0.07178727422021772</v>
       </c>
     </row>
     <row r="68">
@@ -5444,19 +5444,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>3.309171153994266</v>
+        <v>0.10554000962765465</v>
       </c>
       <c r="C4" t="n">
-        <v>2.813859163174303</v>
+        <v>0.09080407478138562</v>
       </c>
       <c r="D4" t="n">
-        <v>2.749461739696509</v>
+        <v>0.08026042888925071</v>
       </c>
       <c r="E4" t="n">
-        <v>2.156578178044747</v>
+        <v>0.0605973937237903</v>
       </c>
       <c r="F4" t="n">
-        <v>2.6754896046500733</v>
+        <v>0.08039428307373746</v>
       </c>
     </row>
     <row r="5">
@@ -5607,19 +5607,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>3.3084703687625705</v>
+        <v>0.09616919462939376</v>
       </c>
       <c r="C13" t="n">
-        <v>3.1361265426576175</v>
+        <v>0.09412460216342948</v>
       </c>
       <c r="D13" t="n">
-        <v>3.869243681593962</v>
+        <v>0.114592634758465</v>
       </c>
       <c r="E13" t="n">
-        <v>2.9737665837809852</v>
+        <v>0.08575897659199197</v>
       </c>
       <c r="F13" t="n">
-        <v>3.372792034311288</v>
+        <v>0.09904437335050192</v>
       </c>
     </row>
     <row r="14">
@@ -5770,19 +5770,19 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>2.9621496673433763</v>
+        <v>0.09938796495585442</v>
       </c>
       <c r="C22" t="n">
-        <v>2.7241818860583495</v>
+        <v>0.09306035389280894</v>
       </c>
       <c r="D22" t="n">
-        <v>2.9785293809381437</v>
+        <v>0.09843276452036434</v>
       </c>
       <c r="E22" t="n">
-        <v>2.4726255822355983</v>
+        <v>0.08235188698692099</v>
       </c>
       <c r="F22" t="n">
-        <v>2.8780306967549536</v>
+        <v>0.0957604560651055</v>
       </c>
     </row>
     <row r="23">
@@ -5933,19 +5933,19 @@
         <v>7</v>
       </c>
       <c r="B31" t="n">
-        <v>3.9604433316938588</v>
+        <v>0.12520064366912328</v>
       </c>
       <c r="C31" t="n">
-        <v>2.8307516347762562</v>
+        <v>0.09115210387255213</v>
       </c>
       <c r="D31" t="n">
-        <v>3.7282354961145794</v>
+        <v>0.11769055338199944</v>
       </c>
       <c r="E31" t="n">
-        <v>3.38350599697417</v>
+        <v>0.10660370663579483</v>
       </c>
       <c r="F31" t="n">
-        <v>3.614689348552626</v>
+        <v>0.11389705478215785</v>
       </c>
     </row>
     <row r="32">
@@ -6096,19 +6096,19 @@
         <v>7</v>
       </c>
       <c r="B40" t="n">
-        <v>4.9094927910886055</v>
+        <v>0.16935592653772386</v>
       </c>
       <c r="C40" t="n">
-        <v>2.3826554633828203</v>
+        <v>0.07225524204310507</v>
       </c>
       <c r="D40" t="n">
-        <v>2.782312448614599</v>
+        <v>0.08743294819037885</v>
       </c>
       <c r="E40" t="n">
-        <v>2.1544632467493923</v>
+        <v>0.061454098998894695</v>
       </c>
       <c r="F40" t="n">
-        <v>3.9793303887115736</v>
+        <v>0.12993389215091425</v>
       </c>
     </row>
     <row r="41">
@@ -6259,19 +6259,19 @@
         <v>7</v>
       </c>
       <c r="B49" t="n">
-        <v>3.6511173636766507</v>
+        <v>0.12360165611901874</v>
       </c>
       <c r="C49" t="n">
-        <v>2.8795176080039813</v>
+        <v>0.09135072648434128</v>
       </c>
       <c r="D49" t="n">
-        <v>2.3286115452517833</v>
+        <v>0.06797601419620826</v>
       </c>
       <c r="E49" t="n">
-        <v>2.1621011828494607</v>
+        <v>0.060166783141012224</v>
       </c>
       <c r="F49" t="n">
-        <v>2.992779782555442</v>
+        <v>0.09304440902788273</v>
       </c>
     </row>
     <row r="50">
@@ -6422,19 +6422,19 @@
         <v>7</v>
       </c>
       <c r="B58" t="n">
-        <v>3.395091637531241</v>
+        <v>0.10566693530211523</v>
       </c>
       <c r="C58" t="n">
-        <v>2.9373984935586597</v>
+        <v>0.09286193862256836</v>
       </c>
       <c r="D58" t="n">
-        <v>3.0730660259369436</v>
+        <v>0.09327290651598795</v>
       </c>
       <c r="E58" t="n">
-        <v>2.5267028599681978</v>
+        <v>0.07483706208819639</v>
       </c>
       <c r="F58" t="n">
-        <v>2.998227966950942</v>
+        <v>0.09226157717424986</v>
       </c>
     </row>
     <row r="59">
@@ -6585,19 +6585,19 @@
         <v>7</v>
       </c>
       <c r="B67" t="n">
-        <v>3.0346231807013244</v>
+        <v>0.09884436140101584</v>
       </c>
       <c r="C67" t="n">
-        <v>2.8568963763332498</v>
+        <v>0.09394784916102124</v>
       </c>
       <c r="D67" t="n">
-        <v>3.1674862607178795</v>
+        <v>0.09920489714758955</v>
       </c>
       <c r="E67" t="n">
-        <v>2.603555516835573</v>
+        <v>0.08233052684173237</v>
       </c>
       <c r="F67" t="n">
-        <v>2.9540594485189042</v>
+        <v>0.09308275466747827</v>
       </c>
     </row>
     <row r="68">
@@ -6761,19 +6761,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>4.23366571085344</v>
+        <v>0.15221515929076462</v>
       </c>
       <c r="C4" t="n">
-        <v>2.971271139639649</v>
+        <v>0.09919208074874897</v>
       </c>
       <c r="D4" t="n">
-        <v>3.444723365620722</v>
+        <v>0.11080531008119346</v>
       </c>
       <c r="E4" t="n">
-        <v>3.411713887897391</v>
+        <v>0.11032298180871852</v>
       </c>
       <c r="F4" t="n">
-        <v>3.3422761421014333</v>
+        <v>0.11056608944283815</v>
       </c>
     </row>
     <row r="5">
@@ -6924,19 +6924,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>5.068392402465126</v>
+        <v>0.18500000298578614</v>
       </c>
       <c r="C13" t="n">
-        <v>2.9659062171322774</v>
+        <v>0.09998991482420393</v>
       </c>
       <c r="D13" t="n">
-        <v>3.6189003336497336</v>
+        <v>0.11669467398025209</v>
       </c>
       <c r="E13" t="n">
-        <v>3.352518177868136</v>
+        <v>0.1013963255869156</v>
       </c>
       <c r="F13" t="n">
-        <v>3.0994009255963113</v>
+        <v>0.10348604749675894</v>
       </c>
     </row>
     <row r="14">
@@ -7087,19 +7087,19 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>4.149106316165739</v>
+        <v>0.1338265319267906</v>
       </c>
       <c r="C22" t="n">
-        <v>3.13881759761065</v>
+        <v>0.09846099065236674</v>
       </c>
       <c r="D22" t="n">
-        <v>3.7725322373074497</v>
+        <v>0.11244088270341464</v>
       </c>
       <c r="E22" t="n">
-        <v>3.601099199839576</v>
+        <v>0.10914994301646626</v>
       </c>
       <c r="F22" t="n">
-        <v>2.9337930476109326</v>
+        <v>0.09165831231063155</v>
       </c>
     </row>
     <row r="23">
@@ -7250,19 +7250,19 @@
         <v>7</v>
       </c>
       <c r="B31" t="n">
-        <v>4.1997825178993</v>
+        <v>0.1435293751960105</v>
       </c>
       <c r="C31" t="n">
-        <v>2.885790064951918</v>
+        <v>0.09094901400408847</v>
       </c>
       <c r="D31" t="n">
-        <v>3.262866137488999</v>
+        <v>0.09732689939701833</v>
       </c>
       <c r="E31" t="n">
-        <v>2.9977923645757873</v>
+        <v>0.08363065255522228</v>
       </c>
       <c r="F31" t="n">
-        <v>3.165598928836836</v>
+        <v>0.09530394301320126</v>
       </c>
     </row>
     <row r="32">
@@ -7413,19 +7413,19 @@
         <v>7</v>
       </c>
       <c r="B40" t="n">
-        <v>5.06559129805086</v>
+        <v>0.1767445157913882</v>
       </c>
       <c r="C40" t="n">
-        <v>2.5726996740504666</v>
+        <v>0.07705714659589896</v>
       </c>
       <c r="D40" t="n">
-        <v>4.053434433306901</v>
+        <v>0.13217134977261716</v>
       </c>
       <c r="E40" t="n">
-        <v>3.026846380656974</v>
+        <v>0.08931997490975804</v>
       </c>
       <c r="F40" t="n">
-        <v>6.1987141488341715</v>
+        <v>0.22286435912538105</v>
       </c>
     </row>
     <row r="41">
@@ -7576,19 +7576,19 @@
         <v>7</v>
       </c>
       <c r="B49" t="n">
-        <v>3.335279781466328</v>
+        <v>0.08305643111701425</v>
       </c>
       <c r="C49" t="n">
-        <v>2.4549140741913607</v>
+        <v>0.06783938769959215</v>
       </c>
       <c r="D49" t="n">
-        <v>3.9389799956201523</v>
+        <v>0.09331966571377806</v>
       </c>
       <c r="E49" t="n">
-        <v>3.675538554811136</v>
+        <v>0.114448328685993</v>
       </c>
       <c r="F49" t="n">
-        <v>7.536902415427884</v>
+        <v>0.2507335862668833</v>
       </c>
     </row>
     <row r="50">
@@ -7739,19 +7739,19 @@
         <v>7</v>
       </c>
       <c r="B58" t="n">
-        <v>4.675770563590342</v>
+        <v>0.16426536965314212</v>
       </c>
       <c r="C58" t="n">
-        <v>3.2264140846149933</v>
+        <v>0.10396883721971266</v>
       </c>
       <c r="D58" t="n">
-        <v>4.2894656348544125</v>
+        <v>0.1367620587187847</v>
       </c>
       <c r="E58" t="n">
-        <v>4.482755535300356</v>
+        <v>0.13343303067176743</v>
       </c>
       <c r="F58" t="n">
-        <v>3.55081662359026</v>
+        <v>0.10682150801380705</v>
       </c>
     </row>
     <row r="59">
@@ -7902,19 +7902,19 @@
         <v>7</v>
       </c>
       <c r="B67" t="n">
-        <v>4.911268765148021</v>
+        <v>0.1617483705574772</v>
       </c>
       <c r="C67" t="n">
-        <v>3.252038503995681</v>
+        <v>0.10289960391186269</v>
       </c>
       <c r="D67" t="n">
-        <v>3.9906956066430848</v>
+        <v>0.12024989686673522</v>
       </c>
       <c r="E67" t="n">
-        <v>3.978479483368459</v>
+        <v>0.11787255138028313</v>
       </c>
       <c r="F67" t="n">
-        <v>3.511036042847419</v>
+        <v>0.11052482721465615</v>
       </c>
     </row>
     <row r="68">
@@ -8078,19 +8078,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>2.3997594548642063</v>
+        <v>0.0769210922584897</v>
       </c>
       <c r="C4" t="n">
-        <v>2.2851320158648347</v>
+        <v>0.07577771727979538</v>
       </c>
       <c r="D4" t="n">
-        <v>2.0108697884149227</v>
+        <v>0.06470025493993256</v>
       </c>
       <c r="E4" t="n">
-        <v>1.9950543803006966</v>
+        <v>0.06320225596094099</v>
       </c>
       <c r="F4" t="n">
-        <v>2.3259536260755604</v>
+        <v>0.07531551054589032</v>
       </c>
     </row>
     <row r="5">
@@ -8241,19 +8241,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>3.372966405030057</v>
+        <v>0.11605487633250561</v>
       </c>
       <c r="C13" t="n">
-        <v>2.4326868991880914</v>
+        <v>0.08285580001561002</v>
       </c>
       <c r="D13" t="n">
-        <v>1.8671730413137315</v>
+        <v>0.05875023639569546</v>
       </c>
       <c r="E13" t="n">
-        <v>1.9406384498747888</v>
+        <v>0.061218471193024135</v>
       </c>
       <c r="F13" t="n">
-        <v>2.448866967742515</v>
+        <v>0.08457383232492632</v>
       </c>
     </row>
     <row r="14">
@@ -8404,19 +8404,19 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>2.0265029016942813</v>
+        <v>0.07168414147483226</v>
       </c>
       <c r="C22" t="n">
-        <v>2.1420167193948694</v>
+        <v>0.07783790695226428</v>
       </c>
       <c r="D22" t="n">
-        <v>1.7256127459023782</v>
+        <v>0.060592185768770374</v>
       </c>
       <c r="E22" t="n">
-        <v>1.946889501704546</v>
+        <v>0.06829165122220654</v>
       </c>
       <c r="F22" t="n">
-        <v>1.96834042612976</v>
+        <v>0.07139852264005092</v>
       </c>
     </row>
     <row r="23">
@@ -8567,19 +8567,19 @@
         <v>7</v>
       </c>
       <c r="B31" t="n">
-        <v>2.3338150282810712</v>
+        <v>0.07774184913467129</v>
       </c>
       <c r="C31" t="n">
-        <v>2.4044023427089676</v>
+        <v>0.07995486788635041</v>
       </c>
       <c r="D31" t="n">
-        <v>1.8393096917925493</v>
+        <v>0.060124255201395874</v>
       </c>
       <c r="E31" t="n">
-        <v>2.1120298372598056</v>
+        <v>0.06674866724683994</v>
       </c>
       <c r="F31" t="n">
-        <v>2.5104053583356856</v>
+        <v>0.08294502131510356</v>
       </c>
     </row>
     <row r="32">
@@ -8730,19 +8730,19 @@
         <v>7</v>
       </c>
       <c r="B40" t="n">
-        <v>4.834030534396873</v>
+        <v>0.18457669045254665</v>
       </c>
       <c r="C40" t="n">
-        <v>2.4998970624782104</v>
+        <v>0.08696015393330699</v>
       </c>
       <c r="D40" t="n">
-        <v>3.783210472797024</v>
+        <v>0.14092511461220433</v>
       </c>
       <c r="E40" t="n">
-        <v>1.1134428981298006</v>
+        <v>0.03603470232076936</v>
       </c>
       <c r="F40" t="n">
-        <v>4.471740433249274</v>
+        <v>0.16763276176082786</v>
       </c>
     </row>
     <row r="41">
@@ -8893,19 +8893,19 @@
         <v>7</v>
       </c>
       <c r="B49" t="n">
-        <v>3.278777470410671</v>
+        <v>0.10875531634458674</v>
       </c>
       <c r="C49" t="n">
-        <v>2.7350503433947906</v>
+        <v>0.08998296378142089</v>
       </c>
       <c r="D49" t="n">
-        <v>1.922975504857419</v>
+        <v>0.05918845775668514</v>
       </c>
       <c r="E49" t="n">
-        <v>1.8929862107575255</v>
+        <v>0.055115237178165154</v>
       </c>
       <c r="F49" t="n">
-        <v>3.7812467179341347</v>
+        <v>0.11834702572212402</v>
       </c>
     </row>
     <row r="50">
@@ -9056,19 +9056,19 @@
         <v>7</v>
       </c>
       <c r="B58" t="n">
-        <v>2.8700941508189617</v>
+        <v>0.09273319471248147</v>
       </c>
       <c r="C58" t="n">
-        <v>2.414640966999529</v>
+        <v>0.07912002677324946</v>
       </c>
       <c r="D58" t="n">
-        <v>2.1297659843985093</v>
+        <v>0.06863116676501393</v>
       </c>
       <c r="E58" t="n">
-        <v>1.9274630827391377</v>
+        <v>0.05847072032074119</v>
       </c>
       <c r="F58" t="n">
-        <v>2.5915410890602284</v>
+        <v>0.0876281636535187</v>
       </c>
     </row>
     <row r="59">
@@ -9219,19 +9219,19 @@
         <v>7</v>
       </c>
       <c r="B67" t="n">
-        <v>2.444914051816823</v>
+        <v>0.07468809789704976</v>
       </c>
       <c r="C67" t="n">
-        <v>2.548776716957037</v>
+        <v>0.0795498842971787</v>
       </c>
       <c r="D67" t="n">
-        <v>2.0235906875439844</v>
+        <v>0.058687701687157305</v>
       </c>
       <c r="E67" t="n">
-        <v>2.2829123450279694</v>
+        <v>0.06528180948007249</v>
       </c>
       <c r="F67" t="n">
-        <v>2.4243985502573473</v>
+        <v>0.0732813993731821</v>
       </c>
     </row>
     <row r="68">

</xml_diff>